<commit_message>
emission activity ratios for electricity generation techs updated
</commit_message>
<xml_diff>
--- a/dashboard/Data/Electricity_generation.xlsx
+++ b/dashboard/Data/Electricity_generation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t>OSEMOSYS</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Renewable</t>
+  </si>
+  <si>
+    <t>EmissionActivityRatio</t>
   </si>
 </sst>
 </file>
@@ -471,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -495,6 +498,9 @@
       <c r="D1" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="E1" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
@@ -511,6 +517,9 @@
       <c r="D2" t="s">
         <v>29</v>
       </c>
+      <c r="E2">
+        <v>9.6100000000000005E-2</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -525,6 +534,9 @@
       <c r="D3" t="s">
         <v>29</v>
       </c>
+      <c r="E3">
+        <v>5.6099999999999997E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -539,6 +551,9 @@
       <c r="D4" t="s">
         <v>29</v>
       </c>
+      <c r="E4">
+        <v>7.4099999999999999E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -553,6 +568,9 @@
       <c r="D5" t="s">
         <v>30</v>
       </c>
+      <c r="E5">
+        <v>0.1225</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -623,6 +641,9 @@
       <c r="D10" t="s">
         <v>29</v>
       </c>
+      <c r="E10">
+        <v>7.4099999999999999E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
@@ -636,6 +657,9 @@
       </c>
       <c r="D11" t="s">
         <v>29</v>
+      </c>
+      <c r="E11">
+        <v>7.4099999999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
fixed CO2 plot, res figures and RE share in elec system title
</commit_message>
<xml_diff>
--- a/dashboard/Data/Electricity_generation.xlsx
+++ b/dashboard/Data/Electricity_generation.xlsx
@@ -474,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -585,6 +585,9 @@
       <c r="D6" t="s">
         <v>30</v>
       </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -599,6 +602,9 @@
       <c r="D7" t="s">
         <v>30</v>
       </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
@@ -613,6 +619,9 @@
       <c r="D8" t="s">
         <v>30</v>
       </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -627,6 +636,9 @@
       <c r="D9" t="s">
         <v>30</v>
       </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
@@ -675,6 +687,9 @@
       <c r="D12" t="s">
         <v>30</v>
       </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
@@ -688,6 +703,9 @@
       </c>
       <c r="D13" t="s">
         <v>30</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>